<commit_message>
baffin bay floats parameters
</commit_message>
<xml_diff>
--- a/docs/Copy of PROG AMUNDSEN ARVOR.xlsx
+++ b/docs/Copy of PROG AMUNDSEN ARVOR.xlsx
@@ -346,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +368,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -539,6 +545,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,11 +832,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -831,10 +842,11 @@
     <col min="2" max="2" width="6.1796875" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.453125" style="1"/>
+    <col min="5" max="5" width="11.453125" style="38"/>
+    <col min="6" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -848,7 +860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>61</v>
       </c>
@@ -860,23 +872,26 @@
       </c>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="36">
         <v>500</v>
       </c>
       <c r="C3" s="7">
         <v>300</v>
       </c>
       <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E3" s="38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="36">
         <v>168</v>
       </c>
       <c r="C4" s="7">
@@ -885,12 +900,15 @@
       <c r="D4" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="38">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="36">
         <v>240</v>
       </c>
       <c r="C5" s="7">
@@ -899,8 +917,11 @@
       <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E5" s="38">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>65</v>
       </c>
@@ -914,7 +935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>66</v>
       </c>
@@ -928,7 +949,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>67</v>
       </c>
@@ -942,7 +963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>68</v>
       </c>
@@ -954,7 +975,7 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>69</v>
       </c>
@@ -968,7 +989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>70</v>
       </c>
@@ -982,7 +1003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>71</v>
       </c>
@@ -996,7 +1017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>72</v>
       </c>
@@ -1010,7 +1031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>73</v>
       </c>
@@ -1024,7 +1045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>74</v>
       </c>
@@ -1038,11 +1059,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16" s="36">
         <v>2000</v>
       </c>
       <c r="C16" s="7">
@@ -1050,6 +1071,9 @@
       </c>
       <c r="D16" s="8" t="s">
         <v>9</v>
+      </c>
+      <c r="E16" s="38">
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1482,7 +1506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>49</v>
       </c>
@@ -1496,7 +1520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>50</v>
       </c>
@@ -1510,7 +1534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>51</v>
       </c>
@@ -1524,7 +1548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>52</v>
       </c>
@@ -1538,7 +1562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>53</v>
       </c>
@@ -1552,7 +1576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>54</v>
       </c>
@@ -1566,7 +1590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>55</v>
       </c>
@@ -1578,7 +1602,7 @@
       </c>
       <c r="D55" s="18"/>
     </row>
-    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>56</v>
       </c>
@@ -1592,7 +1616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>57</v>
       </c>
@@ -1606,7 +1630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>58</v>
       </c>
@@ -1620,7 +1644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>59</v>
       </c>
@@ -1630,7 +1654,7 @@
       </c>
       <c r="D59" s="18"/>
     </row>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="20" t="s">
         <v>60</v>
       </c>
@@ -1640,17 +1664,17 @@
       </c>
       <c r="D60" s="22"/>
     </row>
-    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="23"/>
       <c r="B61" s="26"/>
       <c r="C61" s="24"/>
       <c r="D61" s="25"/>
     </row>
-    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B62" s="34">
+      <c r="B62" s="37">
         <v>10</v>
       </c>
       <c r="C62" s="15">
@@ -1659,8 +1683,11 @@
       <c r="D62" s="16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E62" s="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>20</v>
       </c>
@@ -1674,7 +1701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
         <v>21</v>
       </c>

</xml_diff>